<commit_message>
Finished automation without validation
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/DataBase.xlsx
+++ b/src/main/java/resources/excelsheet/DataBase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>number</t>
   </si>
@@ -163,6 +163,24 @@
   </si>
   <si>
     <t>11,12,13,14,15</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>passportid</t>
+  </si>
+  <si>
+    <t>Gopi,Gowri,Gowreesh,Gopika,Graden</t>
+  </si>
+  <si>
+    <t>Muthu,gopi,gopi,gopi,gopi</t>
+  </si>
+  <si>
+    <t>1234567890,0987654321,6789054321,0987612345,1236547890</t>
   </si>
 </sst>
 </file>
@@ -514,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,9 +565,12 @@
     <col min="25" max="25" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="54.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -634,8 +655,17 @@
       <c r="AB1" t="s">
         <v>41</v>
       </c>
+      <c r="AC1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -719,6 +749,15 @@
       </c>
       <c r="AB2" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>